<commit_message>
Tag 2 und auf 8 Teams erweitert
</commit_message>
<xml_diff>
--- a/Auswertung.xlsx
+++ b/Auswertung.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/dev/git-repos/SpikeRobotTeamChallenge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DAAF004C-03C5-974F-ABA2-C33FD6FD9310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95388FB5-DFC2-274D-88ED-55A92780EE38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26160" yWindow="5460" windowWidth="29920" windowHeight="19660" xr2:uid="{CFF43321-E119-AF4E-8BE5-765C4ECDCC99}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{CFF43321-E119-AF4E-8BE5-765C4ECDCC99}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tag 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tag 2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="19">
   <si>
     <t>Aufgabe</t>
   </si>
@@ -80,13 +81,19 @@
     <t>Gesamt</t>
   </si>
   <si>
-    <t>Bonuspunkte</t>
-  </si>
-  <si>
     <t>Zeit in Sek</t>
   </si>
   <si>
     <t>Bester Lauf</t>
+  </si>
+  <si>
+    <t>Team 7</t>
+  </si>
+  <si>
+    <t>Team 8</t>
+  </si>
+  <si>
+    <t>Zeitpunkte</t>
   </si>
 </sst>
 </file>
@@ -95,7 +102,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0\ \P\u\n\k\t\e"/>
-    <numFmt numFmtId="166" formatCode="0\ \S\e\k"/>
+    <numFmt numFmtId="165" formatCode="0\ \S\e\k"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -358,37 +365,19 @@
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -404,16 +393,34 @@
     <xf numFmtId="164" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -750,298 +757,372 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{957FBF4C-C2F6-F441-A1F7-866791D26BEB}">
-  <dimension ref="A2:M13"/>
+  <dimension ref="A2:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="17" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:13" ht="22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:17" ht="22" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="12" t="s">
+      <c r="E3" s="19"/>
+      <c r="F3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="5" t="s">
+      <c r="G3" s="19"/>
+      <c r="H3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="12" t="s">
+      <c r="I3" s="19"/>
+      <c r="J3" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="5" t="s">
+      <c r="K3" s="19"/>
+      <c r="L3" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="6"/>
-    </row>
-    <row r="4" spans="1:13" ht="22" x14ac:dyDescent="0.3">
+      <c r="M3" s="19"/>
+      <c r="N3" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="19"/>
+      <c r="P3" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3" s="19"/>
+    </row>
+    <row r="4" spans="1:17" ht="22" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="8"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="17" t="s">
+      <c r="B4" s="23"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="21"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="I5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="18" t="s">
+      <c r="K5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="L5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="18" t="s">
+      <c r="M5" s="12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q5" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="13"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="7"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="13"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="7"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="13"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="7"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="13"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="7"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="8"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="6" t="str">
+        <f>IF(B10="","",IF(B10=MIN($B$10,$D$10,$F$10,$H$10,$J$10,$L$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="C11" s="9" t="str">
+        <f>IF(C10="","",IF(C10=MIN($C$10,$E$10,$G$10,$I$10,$K$10,$M$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="D11" s="6" t="str">
+        <f t="shared" ref="D11" si="0">IF(D10="","",IF(D10=MIN($B$10,$D$10,$F$10,$H$10,$J$10,$L$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="E11" s="9" t="str">
+        <f t="shared" ref="E11" si="1">IF(E10="","",IF(E10=MIN($C$10,$E$10,$G$10,$I$10,$K$10,$M$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="F11" s="6" t="str">
+        <f t="shared" ref="F11" si="2">IF(F10="","",IF(F10=MIN($B$10,$D$10,$F$10,$H$10,$J$10,$L$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="G11" s="9" t="str">
+        <f t="shared" ref="G11" si="3">IF(G10="","",IF(G10=MIN($C$10,$E$10,$G$10,$I$10,$K$10,$M$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="H11" s="6" t="str">
+        <f t="shared" ref="H11" si="4">IF(H10="","",IF(H10=MIN($B$10,$D$10,$F$10,$H$10,$J$10,$L$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="I11" s="9" t="str">
+        <f t="shared" ref="I11" si="5">IF(I10="","",IF(I10=MIN($C$10,$E$10,$G$10,$I$10,$K$10,$M$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="J11" s="6" t="str">
+        <f t="shared" ref="J11" si="6">IF(J10="","",IF(J10=MIN($B$10,$D$10,$F$10,$H$10,$J$10,$L$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="K11" s="9" t="str">
+        <f t="shared" ref="K11" si="7">IF(K10="","",IF(K10=MIN($C$10,$E$10,$G$10,$I$10,$K$10,$M$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="L11" s="6" t="str">
+        <f t="shared" ref="L11" si="8">IF(L10="","",IF(L10=MIN($B$10,$D$10,$F$10,$H$10,$J$10,$L$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="M11" s="9" t="str">
+        <f t="shared" ref="M11" si="9">IF(M10="","",IF(M10=MIN($C$10,$E$10,$G$10,$I$10,$K$10,$M$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="N11" s="6" t="str">
+        <f t="shared" ref="N11" si="10">IF(N10="","",IF(N10=MIN($B$10,$D$10,$F$10,$H$10,$J$10,$L$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="O11" s="9" t="str">
+        <f t="shared" ref="O11" si="11">IF(O10="","",IF(O10=MIN($C$10,$E$10,$G$10,$I$10,$K$10,$M$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="P11" s="6" t="str">
+        <f t="shared" ref="P11" si="12">IF(P10="","",IF(P10=MIN($B$10,$D$10,$F$10,$H$10,$J$10,$L$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="Q11" s="9" t="str">
+        <f t="shared" ref="Q11" si="13">IF(Q10="","",IF(Q10=MIN($C$10,$E$10,$G$10,$I$10,$K$10,$M$10),10,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="15">
+        <f>SUM(B6:B9,B11)</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="16">
+        <f t="shared" ref="C12:M12" si="14">SUM(C6:C9,C11)</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="15">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="16">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="16">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="15">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="16">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="16">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="15">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="16">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="17">
+        <f t="shared" ref="N12:Q12" si="15">SUM(N6:N9,N11)</f>
+        <v>0</v>
+      </c>
+      <c r="O12" s="16">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="P12" s="15">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="16">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="23" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="14" t="s">
         <v>15</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="14"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="11" t="str">
-        <f>IF(B10="","",IF(B10=MIN($B$10,$D$10,$F$10,$H$10,$J$10,$L$10),10,0))</f>
-        <v/>
-      </c>
-      <c r="C11" s="15" t="str">
-        <f>IF(C10="","",IF(C10=MIN($C$10,$E$10,$G$10,$I$10,$K$10,$M$10),10,0))</f>
-        <v/>
-      </c>
-      <c r="D11" s="11" t="str">
-        <f t="shared" ref="D11" si="0">IF(D10="","",IF(D10=MIN($B$10,$D$10,$F$10,$H$10,$J$10,$L$10),10,0))</f>
-        <v/>
-      </c>
-      <c r="E11" s="15" t="str">
-        <f t="shared" ref="E11" si="1">IF(E10="","",IF(E10=MIN($C$10,$E$10,$G$10,$I$10,$K$10,$M$10),10,0))</f>
-        <v/>
-      </c>
-      <c r="F11" s="11" t="str">
-        <f t="shared" ref="F11" si="2">IF(F10="","",IF(F10=MIN($B$10,$D$10,$F$10,$H$10,$J$10,$L$10),10,0))</f>
-        <v/>
-      </c>
-      <c r="G11" s="15" t="str">
-        <f t="shared" ref="G11" si="3">IF(G10="","",IF(G10=MIN($C$10,$E$10,$G$10,$I$10,$K$10,$M$10),10,0))</f>
-        <v/>
-      </c>
-      <c r="H11" s="11" t="str">
-        <f t="shared" ref="H11" si="4">IF(H10="","",IF(H10=MIN($B$10,$D$10,$F$10,$H$10,$J$10,$L$10),10,0))</f>
-        <v/>
-      </c>
-      <c r="I11" s="15" t="str">
-        <f t="shared" ref="I11" si="5">IF(I10="","",IF(I10=MIN($C$10,$E$10,$G$10,$I$10,$K$10,$M$10),10,0))</f>
-        <v/>
-      </c>
-      <c r="J11" s="11" t="str">
-        <f t="shared" ref="J11" si="6">IF(J10="","",IF(J10=MIN($B$10,$D$10,$F$10,$H$10,$J$10,$L$10),10,0))</f>
-        <v/>
-      </c>
-      <c r="K11" s="15" t="str">
-        <f t="shared" ref="K11" si="7">IF(K10="","",IF(K10=MIN($C$10,$E$10,$G$10,$I$10,$K$10,$M$10),10,0))</f>
-        <v/>
-      </c>
-      <c r="L11" s="11" t="str">
-        <f t="shared" ref="L11" si="8">IF(L10="","",IF(L10=MIN($B$10,$D$10,$F$10,$H$10,$J$10,$L$10),10,0))</f>
-        <v/>
-      </c>
-      <c r="M11" s="15" t="str">
-        <f t="shared" ref="M11" si="9">IF(M10="","",IF(M10=MIN($C$10,$E$10,$G$10,$I$10,$K$10,$M$10),10,0))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="21">
-        <f>SUM(B6:B9,B11)</f>
-        <v>0</v>
-      </c>
-      <c r="C12" s="22">
-        <f t="shared" ref="C12:M12" si="10">SUM(C6:C9,C11)</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="21">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="22">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="23">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="22">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="21">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="22">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="23">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="K12" s="22">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="L12" s="21">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="M12" s="22">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="23" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="20" t="s">
-        <v>16</v>
       </c>
       <c r="B13" s="24">
         <f>MAX(B12:C12)</f>
@@ -1049,33 +1130,51 @@
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="24">
-        <f t="shared" ref="D13" si="11">MAX(D12:E12)</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="27"/>
-      <c r="F13" s="26">
-        <f t="shared" ref="F13" si="12">MAX(F12:G12)</f>
+        <f t="shared" ref="D13" si="16">MAX(D12:E12)</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="26"/>
+      <c r="F13" s="27">
+        <f t="shared" ref="F13" si="17">MAX(F12:G12)</f>
         <v>0</v>
       </c>
       <c r="G13" s="25"/>
       <c r="H13" s="24">
-        <f t="shared" ref="H13" si="13">MAX(H12:I12)</f>
-        <v>0</v>
-      </c>
-      <c r="I13" s="27"/>
-      <c r="J13" s="26">
-        <f t="shared" ref="J13" si="14">MAX(J12:K12)</f>
+        <f t="shared" ref="H13" si="18">MAX(H12:I12)</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="26"/>
+      <c r="J13" s="27">
+        <f t="shared" ref="J13" si="19">MAX(J12:K12)</f>
         <v>0</v>
       </c>
       <c r="K13" s="25"/>
       <c r="L13" s="24">
-        <f t="shared" ref="L13" si="15">MAX(L12:M12)</f>
-        <v>0</v>
-      </c>
-      <c r="M13" s="27"/>
+        <f t="shared" ref="L13" si="20">MAX(L12:M12)</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="26"/>
+      <c r="N13" s="27">
+        <f t="shared" ref="N13" si="21">MAX(N12:O12)</f>
+        <v>0</v>
+      </c>
+      <c r="O13" s="25"/>
+      <c r="P13" s="24">
+        <f t="shared" ref="P13" si="22">MAX(P12:Q12)</f>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="24">
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="P4:Q4"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="L3:M3"/>
@@ -1092,11 +1191,9 @@
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="B4:C4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D10 B10 F10 H10 J10 L10">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="B10 D10 F10 H10 J10 L10">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1107,7 +1204,29 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10 E10 G10 I10 K10 M10">
+  <conditionalFormatting sqref="B13:Q13">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10 C10 G10 I10 K10 M10">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P10 N10">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1119,8 +1238,477 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13:M13">
+  <conditionalFormatting sqref="O10 Q10">
     <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B12:M12" formulaRange="1"/>
+    <ignoredError sqref="B11:N11 P11" formula="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C72C74A9-B800-8C42-B98D-76DBCD09CDC8}">
+  <dimension ref="A2:Q13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="17" width="11.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:17" ht="22" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="19"/>
+      <c r="F3" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="19"/>
+      <c r="H3" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="19"/>
+      <c r="J3" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="19"/>
+      <c r="L3" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="19"/>
+      <c r="N3" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="19"/>
+      <c r="P3" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3" s="19"/>
+    </row>
+    <row r="4" spans="1:17" ht="22" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="21"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q5" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="7"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="7"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="7"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="7"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="8"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="6" t="str">
+        <f>IF(B10="","",IF(B10=MIN($B$10,$D$10,$F$10,$H$10,$J$10,$L$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="C11" s="9" t="str">
+        <f>IF(C10="","",IF(C10=MIN($C$10,$E$10,$G$10,$I$10,$K$10,$M$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="D11" s="6" t="str">
+        <f t="shared" ref="D11" si="0">IF(D10="","",IF(D10=MIN($B$10,$D$10,$F$10,$H$10,$J$10,$L$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="E11" s="9" t="str">
+        <f t="shared" ref="E11" si="1">IF(E10="","",IF(E10=MIN($C$10,$E$10,$G$10,$I$10,$K$10,$M$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="F11" s="6" t="str">
+        <f t="shared" ref="F11" si="2">IF(F10="","",IF(F10=MIN($B$10,$D$10,$F$10,$H$10,$J$10,$L$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="G11" s="9" t="str">
+        <f t="shared" ref="G11" si="3">IF(G10="","",IF(G10=MIN($C$10,$E$10,$G$10,$I$10,$K$10,$M$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="H11" s="6" t="str">
+        <f t="shared" ref="H11" si="4">IF(H10="","",IF(H10=MIN($B$10,$D$10,$F$10,$H$10,$J$10,$L$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="I11" s="9" t="str">
+        <f t="shared" ref="I11" si="5">IF(I10="","",IF(I10=MIN($C$10,$E$10,$G$10,$I$10,$K$10,$M$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="J11" s="6" t="str">
+        <f t="shared" ref="J11" si="6">IF(J10="","",IF(J10=MIN($B$10,$D$10,$F$10,$H$10,$J$10,$L$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="K11" s="9" t="str">
+        <f t="shared" ref="K11" si="7">IF(K10="","",IF(K10=MIN($C$10,$E$10,$G$10,$I$10,$K$10,$M$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="L11" s="6" t="str">
+        <f t="shared" ref="L11" si="8">IF(L10="","",IF(L10=MIN($B$10,$D$10,$F$10,$H$10,$J$10,$L$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="M11" s="9" t="str">
+        <f t="shared" ref="M11" si="9">IF(M10="","",IF(M10=MIN($C$10,$E$10,$G$10,$I$10,$K$10,$M$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="N11" s="6" t="str">
+        <f t="shared" ref="N11" si="10">IF(N10="","",IF(N10=MIN($B$10,$D$10,$F$10,$H$10,$J$10,$L$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="O11" s="9" t="str">
+        <f t="shared" ref="O11" si="11">IF(O10="","",IF(O10=MIN($C$10,$E$10,$G$10,$I$10,$K$10,$M$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="P11" s="6" t="str">
+        <f t="shared" ref="P11" si="12">IF(P10="","",IF(P10=MIN($B$10,$D$10,$F$10,$H$10,$J$10,$L$10),10,0))</f>
+        <v/>
+      </c>
+      <c r="Q11" s="9" t="str">
+        <f t="shared" ref="Q11" si="13">IF(Q10="","",IF(Q10=MIN($C$10,$E$10,$G$10,$I$10,$K$10,$M$10),10,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="15">
+        <f>SUM(B6:B9,B11)</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="16">
+        <f t="shared" ref="C12:Q12" si="14">SUM(C6:C9,C11)</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="15">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="16">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="16">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="15">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="16">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="16">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="15">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="16">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="16">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="P12" s="15">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="16">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="23" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="24">
+        <f>MAX(B12:C12)</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="24">
+        <f t="shared" ref="D13" si="15">MAX(D12:E12)</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="26"/>
+      <c r="F13" s="27">
+        <f t="shared" ref="F13" si="16">MAX(F12:G12)</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="25"/>
+      <c r="H13" s="24">
+        <f t="shared" ref="H13" si="17">MAX(H12:I12)</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="26"/>
+      <c r="J13" s="27">
+        <f t="shared" ref="J13" si="18">MAX(J12:K12)</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="25"/>
+      <c r="L13" s="24">
+        <f t="shared" ref="L13" si="19">MAX(L12:M12)</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="26"/>
+      <c r="N13" s="27">
+        <f t="shared" ref="N13" si="20">MAX(N12:O12)</f>
+        <v>0</v>
+      </c>
+      <c r="O13" s="25"/>
+      <c r="P13" s="24">
+        <f t="shared" ref="P13" si="21">MAX(P12:Q12)</f>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="26"/>
+    </row>
+  </sheetData>
+  <mergeCells count="24">
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B10 D10 F10 H10 J10 L10">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:Q13">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1129,10 +1717,45 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E10 C10 G10 I10 K10 M10">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P10 N10">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O10 Q10">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B12:M12" formulaRange="1"/>
-    <ignoredError sqref="B11:M11" formula="1"/>
+    <ignoredError sqref="C11 E11 G11 I11 K11 M11 O11" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>